<commit_message>
Support shared formulas bugfix function DATE and improve tests.
Co-Authored-By: Bradley van Ree <bradbase@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/tests/resources/DATE.xlsx
+++ b/tests/resources/DATE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradb\Documents\Python\koala_xlcalculator\tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF8BEA5-5396-4932-B876-B02D1706FF19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAB4970-11B0-4ED0-962E-4A92C18D46E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2573" yWindow="780" windowWidth="14647" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5205" yWindow="0" windowWidth="14647" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Year</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>Day</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
   <si>
     <t>2016</t>
@@ -364,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -403,7 +406,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
-        <f t="shared" ref="A3" si="0">DATE(B3,C3,D3)</f>
+        <f t="shared" ref="A3:A17" si="0">DATE(B3,C3,D3)</f>
         <v>39755</v>
       </c>
       <c r="B3">
@@ -416,9 +419,54 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" s="1">
+        <f t="shared" si="0"/>
+        <v>45292</v>
+      </c>
+      <c r="B4">
+        <v>2024</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" s="1">
+        <f t="shared" si="0"/>
+        <v>45658</v>
+      </c>
+      <c r="B5">
+        <v>2025</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
+        <v>46023</v>
+      </c>
+      <c r="B6">
+        <v>2026</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
-        <f t="shared" ref="A7" si="1">DATE(B7,C7,D7)</f>
+        <f t="shared" si="0"/>
         <v>39507</v>
       </c>
       <c r="B7">
@@ -431,9 +479,24 @@
         <v>29</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" s="1">
+        <f t="shared" si="0"/>
+        <v>40213</v>
+      </c>
+      <c r="B8">
+        <v>2009</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>400</v>
+      </c>
+    </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
-        <f t="shared" ref="A9" si="2">DATE(B9,C9,D9)</f>
+        <f t="shared" si="0"/>
         <v>40210</v>
       </c>
       <c r="B9">
@@ -446,13 +509,118 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" s="1">
+        <f t="shared" si="0"/>
+        <v>39812</v>
+      </c>
+      <c r="B10">
+        <v>2009</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" s="1">
+        <f t="shared" si="0"/>
+        <v>39753</v>
+      </c>
+      <c r="B11">
+        <v>2009</v>
+      </c>
+      <c r="C11">
+        <v>-1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="B12">
+        <v>1900</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="B13">
+        <v>10000</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="B14">
+        <v>-1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" s="1">
+        <f t="shared" si="0"/>
+        <v>42370</v>
+      </c>
+      <c r="B15">
+        <v>2016</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A16" s="1">
+        <f t="shared" si="0"/>
+        <v>42370</v>
+      </c>
+      <c r="B16">
+        <v>2016</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
-        <f t="shared" ref="A17" si="3">DATE(B17,C17,D17)</f>
+        <f t="shared" si="0"/>
         <v>42370</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -461,16 +629,102 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <f>DATE(2000, 1, 1)</f>
         <v>36526</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <f>DATE("2000",1, 1)</f>
         <v>36526</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>5</v>
+      </c>
+      <c r="F24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" s="1">
+        <f>DATE(A24,A23,A22)</f>
+        <v>367</v>
+      </c>
+      <c r="B25" s="1">
+        <f t="shared" ref="B25:F25" si="1">DATE(B24,B23,B22)</f>
+        <v>732</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" si="1"/>
+        <v>1097</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="1"/>
+        <v>1462</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="1"/>
+        <v>1828</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="1"/>
+        <v>2193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>